<commit_message>
add register , faker lib
</commit_message>
<xml_diff>
--- a/src/test/java/data/DataYodyfile.xlsx
+++ b/src/test/java/data/DataYodyfile.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet5" sheetId="5" r:id="rId4"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId5"/>
+    <sheet name="register" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="133">
   <si>
     <t>username</t>
   </si>
@@ -394,180 +394,15 @@
     <t>Kiểm tra đăng kí thành công</t>
   </si>
   <si>
-    <t xml:space="preserve">random </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kiểm tra đăng kí thành công với số điện thoại chứa +84 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nhập số điện thoại dưới 10 chữ số </t>
-  </si>
-  <si>
-    <t>Nhập số điện thoại trên 10 chữ số</t>
-  </si>
-  <si>
-    <t>Nhập số điện thoại đủ 10 số nhưng không bao gồm số 0 ở đầu</t>
-  </si>
-  <si>
-    <t>Nhập số điện thoại là 1 dãy số liên tiếp 0123456789</t>
-  </si>
-  <si>
-    <t>Nhập SĐT  là chữ</t>
-  </si>
-  <si>
-    <t>Nhập SĐT  là ký tự đặc biệt</t>
-  </si>
-  <si>
-    <t>Nhập SĐT  là số âm</t>
-  </si>
-  <si>
-    <t>Nhập SĐT  là số thập phân</t>
-  </si>
-  <si>
-    <t>Nhập SĐT  là toàn số 0</t>
-  </si>
-  <si>
-    <t>Nhập SĐT có chưa khoảng trắng ở giữa</t>
-  </si>
-  <si>
-    <t>Nhập SĐT có chưa khoảng trắng ở đầu và cuối</t>
-  </si>
-  <si>
-    <t>091923456</t>
-  </si>
-  <si>
-    <t>0919234563434</t>
-  </si>
-  <si>
-    <t>0123456789</t>
-  </si>
-  <si>
-    <t>@*))</t>
-  </si>
-  <si>
-    <t>0000000000</t>
-  </si>
-  <si>
-    <t>random số điện thoại có khoảng trắng ở giữa</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
     <t>random</t>
   </si>
   <si>
-    <t xml:space="preserve">Nhập họ tên không phân biệt hoa thường </t>
-  </si>
-  <si>
-    <t>ThUy THuy</t>
-  </si>
-  <si>
-    <t>ThUy Thuy 123435</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nhập họ tên có chứa số  </t>
-  </si>
-  <si>
-    <t>ThUy Thuy Tester</t>
-  </si>
-  <si>
-    <t>0962351771</t>
-  </si>
-  <si>
-    <t>thuytest238829@gmail.com</t>
-  </si>
-  <si>
     <t>TC19</t>
   </si>
   <si>
-    <t>Nhập mật khẩu và refresh</t>
-  </si>
-  <si>
-    <t>TC20</t>
-  </si>
-  <si>
-    <t>thuythuyrandom</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 123456</t>
-  </si>
-  <si>
-    <t>Nhập mật khẩu có dấu cách</t>
-  </si>
-  <si>
-    <t>thuyrandom</t>
-  </si>
-  <si>
-    <t>TC21</t>
-  </si>
-  <si>
-    <t>thuyrandom23@tester.com</t>
-  </si>
-  <si>
-    <t>TC22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thuy Nguyen </t>
-  </si>
-  <si>
-    <t>Bỏ trống họ tên</t>
-  </si>
-  <si>
-    <t>Bỏ trống email</t>
-  </si>
-  <si>
-    <t>Nhập email trùng trong hệ thống</t>
-  </si>
-  <si>
-    <t>TC23</t>
-  </si>
-  <si>
-    <t>Nhập email thiếu kí tự như (@,.com)</t>
-  </si>
-  <si>
-    <t>testerht.com</t>
-  </si>
-  <si>
-    <t>TC24</t>
-  </si>
-  <si>
-    <t>Nhập email toàn là kí tự đặc biệt</t>
-  </si>
-  <si>
-    <t>#$%^&amp;*(</t>
-  </si>
-  <si>
-    <t>spaceradom</t>
-  </si>
-  <si>
-    <t>TC25</t>
-  </si>
-  <si>
-    <t>TC26</t>
-  </si>
-  <si>
-    <t>TC27</t>
-  </si>
-  <si>
-    <t xml:space="preserve">         Thuy     Nguyen    Space   </t>
-  </si>
-  <si>
-    <t>thuythuy12353456@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    0944561324     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nhập họ và tên và bấm refresh </t>
-  </si>
-  <si>
-    <t>Nhập email bao gồm khoảng trắng đầu cuối</t>
-  </si>
-  <si>
-    <t>Nhập email bao gồm khoảng trắng</t>
-  </si>
-  <si>
     <t xml:space="preserve">Bỏ trống trường địa chỉ giao hàng </t>
   </si>
   <si>
@@ -578,6 +413,15 @@
   </si>
   <si>
     <t>tester2943865306@gmail.</t>
+  </si>
+  <si>
+    <t>Tester Nguyễn</t>
+  </si>
+  <si>
+    <t>automation</t>
+  </si>
+  <si>
+    <t>01292394</t>
   </si>
 </sst>
 </file>
@@ -667,7 +511,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -687,11 +531,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1020,13 +861,13 @@
         <v>38</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>184</v>
+        <v>129</v>
       </c>
       <c r="C3" s="1">
         <v>123456</v>
       </c>
-      <c r="D3" s="15" t="s">
-        <v>183</v>
+      <c r="D3" s="11" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -1043,7 +884,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -1374,7 +1215,7 @@
         <v>73</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>181</v>
+        <v>126</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>2</v>
@@ -1866,7 +1707,7 @@
         <v>116</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>182</v>
+        <v>127</v>
       </c>
       <c r="C18" s="10" t="s">
         <v>103</v>
@@ -1939,7 +1780,7 @@
     </row>
     <row r="20" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>151</v>
+        <v>125</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>86</v>
@@ -2206,10 +2047,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2225,7 +2066,7 @@
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>142</v>
+        <v>123</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>120</v>
@@ -2245,13 +2086,13 @@
         <v>72</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>113</v>
+        <v>130</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>154</v>
+        <v>131</v>
       </c>
       <c r="E2" s="1">
         <v>123456</v>
@@ -2261,501 +2102,15 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="E3" s="1">
-        <v>123456</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="E4" s="1">
-        <v>123456</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>137</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="E5" s="1">
-        <v>123456</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C6" s="1">
-        <v>9294458485</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="E6" s="1">
-        <v>123456</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>138</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="E7" s="1">
-        <v>123456</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="E8" s="1">
-        <v>123456</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>139</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="E9" s="1">
-        <v>123456</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C10" s="1">
-        <v>-139495</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="E10" s="1">
-        <v>123456</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C11" s="1">
-        <v>12324.923040199999</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="E11" s="1">
-        <v>123456</v>
-      </c>
-      <c r="F11" s="1" t="s">
+      <c r="C3" s="12" t="s">
         <v>132</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>140</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="E12" s="1">
-        <v>123456</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="E13" s="1">
-        <v>123456</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>177</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="E14" s="1">
-        <v>123456</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="E15" s="1">
-        <v>123456</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="E16" s="1">
-        <v>123456</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C17" s="11"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>149</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="B19" s="1"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="1">
-        <v>1223456</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>149</v>
-      </c>
-      <c r="D20" s="13" t="s">
-        <v>157</v>
-      </c>
-      <c r="E20" s="12" t="s">
-        <v>155</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="B21" s="1"/>
-      <c r="C21" s="11" t="s">
-        <v>149</v>
-      </c>
-      <c r="D21" s="13" t="s">
-        <v>159</v>
-      </c>
-      <c r="E21" s="12" t="s">
-        <v>155</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="C22" s="14" t="s">
-        <v>149</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E22" s="1">
-        <v>123456</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="C23" s="14" t="s">
-        <v>149</v>
-      </c>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1">
-        <v>123456</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="C24" s="14" t="s">
-        <v>149</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="E24" s="1">
-        <v>123456</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="C25" s="14" t="s">
-        <v>149</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="E25" s="1">
-        <v>123456</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="E26" s="1">
-        <v>123456</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="B27" s="14" t="s">
-        <v>175</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="E27" s="1">
-        <v>123456</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>180</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" display="thuythuy1235@gmail.com"/>
-    <hyperlink ref="D3" r:id="rId2" display="thuythuy1235@gmail.com"/>
-    <hyperlink ref="D4" r:id="rId3"/>
-    <hyperlink ref="D15" r:id="rId4" display="thuythuy1235@gmail.com"/>
-    <hyperlink ref="D16" r:id="rId5" display="thuythuy1235@gmail.com"/>
-    <hyperlink ref="D18" r:id="rId6"/>
-    <hyperlink ref="D20" r:id="rId7" display="thuy272348@gmail.com"/>
-    <hyperlink ref="D21" r:id="rId8"/>
-    <hyperlink ref="D22" r:id="rId9"/>
-    <hyperlink ref="D5:D14" r:id="rId10" display="thuythuy12353456@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId11"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>